<commit_message>
WW Data import cont.
</commit_message>
<xml_diff>
--- a/data/Updated/Sydney Water wet weather intensive.xlsx
+++ b/data/Updated/Sydney Water wet weather intensive.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github 2018\Hawkesbury\data\Updated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Hawkesbury\data\Updated\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5486CA7F-36FD-43B3-8A72-F75F29724D55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12020" tabRatio="940" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-4200" windowWidth="16440" windowHeight="28590" tabRatio="940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wet weather Nov 2018" sheetId="9" r:id="rId1"/>
@@ -20,23 +21,31 @@
   <externalReferences>
     <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Merran Griffith</author>
   </authors>
   <commentList>
-    <comment ref="BG118" authorId="0" shapeId="0">
+    <comment ref="BG118" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -3076,7 +3085,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -4648,7 +4657,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5212,7 +5220,6 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5333,7 +5340,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5408,7 +5414,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -5416,6 +5421,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5490,7 +5496,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6585,7 +6590,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6706,7 +6710,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6781,7 +6784,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6813,7 +6815,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -6821,6 +6822,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -6900,7 +6902,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7995,7 +7996,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8110,7 +8110,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8185,7 +8184,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8217,7 +8215,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -8225,6 +8222,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -10124,7 +10122,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -10132,6 +10129,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -11420,7 +11418,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -11428,6 +11425,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -12204,7 +12202,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -12212,6 +12209,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -12933,7 +12931,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -12941,6 +12938,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -13687,7 +13685,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -13695,6 +13692,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -14416,7 +14414,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -14424,6 +14421,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -20919,52 +20917,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO127"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110:D111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.1796875" customWidth="1"/>
-    <col min="2" max="2" width="38.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="19.26953125" style="32" customWidth="1"/>
-    <col min="6" max="6" width="45.26953125" style="32" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="32" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" style="32" customWidth="1"/>
-    <col min="10" max="10" width="22.1796875" style="32" customWidth="1"/>
-    <col min="11" max="11" width="22.7265625" style="32" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" style="32" customWidth="1"/>
-    <col min="13" max="13" width="12.26953125" style="32" customWidth="1"/>
-    <col min="14" max="14" width="22.1796875" style="32" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.453125" style="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="32" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="32" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="32" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="32" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="32" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="32" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="32" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="32" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" style="32" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.26953125" style="32" customWidth="1"/>
-    <col min="19" max="19" width="19.26953125" style="32" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.28515625" style="32" customWidth="1"/>
+    <col min="19" max="19" width="19.28515625" style="32" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="19" customWidth="1"/>
     <col min="21" max="21" width="16" style="32" customWidth="1"/>
-    <col min="22" max="22" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.54296875" style="32" customWidth="1"/>
-    <col min="24" max="24" width="14.7265625" style="159" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.54296875" style="32" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.5703125" style="32" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" style="159" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.5703125" style="32" customWidth="1"/>
     <col min="26" max="26" width="19" style="32" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="19" style="32" customWidth="1"/>
-    <col min="28" max="28" width="20.26953125" style="32" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.1796875" style="32" customWidth="1"/>
-    <col min="34" max="34" width="10.1796875" customWidth="1"/>
-    <col min="35" max="35" width="22.54296875" customWidth="1"/>
-    <col min="36" max="36" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.140625" style="32" customWidth="1"/>
+    <col min="34" max="34" width="10.140625" customWidth="1"/>
+    <col min="35" max="35" width="22.5703125" customWidth="1"/>
+    <col min="36" max="36" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="114" customFormat="1" ht="18.25" customHeight="1">
+    <row r="1" spans="1:40" s="114" customFormat="1" ht="18.2" customHeight="1">
       <c r="A1" s="28" t="s">
         <v>2</v>
       </c>
@@ -21067,7 +21065,7 @@
       <c r="AM1" s="140"/>
       <c r="AN1" s="140"/>
     </row>
-    <row r="2" spans="1:40" s="114" customFormat="1" ht="18.25" customHeight="1">
+    <row r="2" spans="1:40" s="114" customFormat="1" ht="18.2" customHeight="1">
       <c r="A2" s="28"/>
       <c r="B2" s="27"/>
       <c r="C2" s="112"/>
@@ -21156,7 +21154,7 @@
       <c r="AJ2" s="128"/>
       <c r="AK2" s="128"/>
     </row>
-    <row r="3" spans="1:40" s="114" customFormat="1" ht="18.25" customHeight="1">
+    <row r="3" spans="1:40" s="114" customFormat="1" ht="18.2" customHeight="1">
       <c r="A3" s="28"/>
       <c r="B3" s="27"/>
       <c r="C3" s="116" t="s">
@@ -21247,7 +21245,7 @@
       <c r="AJ3" s="128"/>
       <c r="AK3" s="128"/>
     </row>
-    <row r="4" spans="1:40" s="114" customFormat="1" ht="18.25" customHeight="1">
+    <row r="4" spans="1:40" s="114" customFormat="1" ht="18.2" customHeight="1">
       <c r="A4" s="28"/>
       <c r="B4" s="27" t="s">
         <v>883</v>
@@ -23567,7 +23565,7 @@
       <c r="AJ49" s="143"/>
       <c r="AK49" s="143"/>
     </row>
-    <row r="50" spans="1:37" s="114" customFormat="1" ht="28.75" customHeight="1">
+    <row r="50" spans="1:37" s="114" customFormat="1" ht="28.7" customHeight="1">
       <c r="A50" s="3">
         <v>44</v>
       </c>
@@ -28434,7 +28432,7 @@
       <c r="C110" s="117" t="s">
         <v>781</v>
       </c>
-      <c r="D110" s="117">
+      <c r="D110" s="118">
         <v>43433</v>
       </c>
       <c r="E110" s="117" t="s">
@@ -28551,7 +28549,7 @@
       <c r="C111" s="117" t="s">
         <v>777</v>
       </c>
-      <c r="D111" s="117">
+      <c r="D111" s="118">
         <v>43433</v>
       </c>
       <c r="E111" s="117" t="s">
@@ -29448,103 +29446,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="BD89" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.26953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.7265625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="9.1796875" style="1"/>
-    <col min="26" max="26" width="37.26953125" style="16" customWidth="1"/>
-    <col min="27" max="27" width="8.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="1"/>
+    <col min="26" max="26" width="37.28515625" style="16" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="30" max="33" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="40" max="42" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.7265625" style="32" customWidth="1"/>
+    <col min="43" max="43" width="11.7109375" style="32" customWidth="1"/>
     <col min="44" max="44" width="46" style="51" customWidth="1"/>
     <col min="45" max="45" width="12" style="32" customWidth="1"/>
     <col min="46" max="46" width="28" style="32" customWidth="1"/>
-    <col min="47" max="47" width="14.26953125" style="32" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.453125" style="32" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.7265625" style="32" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.1796875" style="32"/>
-    <col min="51" max="51" width="14.26953125" style="32" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.1796875" style="32" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.7265625" style="32" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.1796875" style="32"/>
-    <col min="55" max="55" width="16.7265625" style="32" customWidth="1"/>
-    <col min="56" max="56" width="37.453125" style="45" customWidth="1"/>
-    <col min="57" max="57" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="37.26953125" style="3" customWidth="1"/>
-    <col min="59" max="59" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.140625" style="32"/>
+    <col min="51" max="51" width="14.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.140625" style="32"/>
+    <col min="55" max="55" width="16.7109375" style="32" customWidth="1"/>
+    <col min="56" max="56" width="37.42578125" style="45" customWidth="1"/>
+    <col min="57" max="57" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="37.28515625" style="3" customWidth="1"/>
+    <col min="59" max="59" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.1796875" style="3" customWidth="1"/>
-    <col min="63" max="63" width="9.1796875" style="3"/>
-    <col min="64" max="64" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8.7265625"/>
-    <col min="69" max="69" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="37.26953125" style="1" customWidth="1"/>
-    <col min="71" max="71" width="23.453125" style="3" customWidth="1"/>
-    <col min="72" max="72" width="61.1796875" style="3" customWidth="1"/>
-    <col min="73" max="73" width="47.81640625" style="1" customWidth="1"/>
-    <col min="74" max="80" width="9.1796875" style="1"/>
-    <col min="81" max="81" width="15.453125" customWidth="1"/>
-    <col min="82" max="83" width="8.7265625"/>
-    <col min="84" max="85" width="9.1796875" style="1"/>
-    <col min="86" max="86" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="34.26953125" style="1" customWidth="1"/>
-    <col min="88" max="88" width="28.81640625" style="1" customWidth="1"/>
+    <col min="62" max="62" width="14.140625" style="3" customWidth="1"/>
+    <col min="63" max="63" width="9.140625" style="3"/>
+    <col min="64" max="64" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8.7109375"/>
+    <col min="69" max="69" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="37.28515625" style="1" customWidth="1"/>
+    <col min="71" max="71" width="23.42578125" style="3" customWidth="1"/>
+    <col min="72" max="72" width="61.140625" style="3" customWidth="1"/>
+    <col min="73" max="73" width="47.85546875" style="1" customWidth="1"/>
+    <col min="74" max="80" width="9.140625" style="1"/>
+    <col min="81" max="81" width="15.42578125" customWidth="1"/>
+    <col min="82" max="83" width="8.7109375"/>
+    <col min="84" max="85" width="9.140625" style="1"/>
+    <col min="86" max="86" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="34.28515625" style="1" customWidth="1"/>
+    <col min="88" max="88" width="28.85546875" style="1" customWidth="1"/>
     <col min="89" max="89" width="15" style="3" customWidth="1"/>
-    <col min="90" max="91" width="9.1796875" style="3"/>
-    <col min="92" max="92" width="8.7265625"/>
-    <col min="93" max="93" width="13.81640625" style="1" customWidth="1"/>
-    <col min="94" max="94" width="11.26953125" style="3" customWidth="1"/>
-    <col min="95" max="97" width="9.1796875" style="3"/>
-    <col min="98" max="98" width="15.7265625" style="1" customWidth="1"/>
-    <col min="99" max="99" width="9.1796875" style="3"/>
-    <col min="100" max="100" width="9.1796875" style="1"/>
-    <col min="101" max="101" width="9.1796875" style="96"/>
-    <col min="102" max="16384" width="9.1796875" style="1"/>
+    <col min="90" max="91" width="9.140625" style="3"/>
+    <col min="92" max="92" width="8.7109375"/>
+    <col min="93" max="93" width="13.85546875" style="1" customWidth="1"/>
+    <col min="94" max="94" width="11.28515625" style="3" customWidth="1"/>
+    <col min="95" max="97" width="9.140625" style="3"/>
+    <col min="98" max="98" width="15.7109375" style="1" customWidth="1"/>
+    <col min="99" max="99" width="9.140625" style="3"/>
+    <col min="100" max="100" width="9.140625" style="1"/>
+    <col min="101" max="101" width="9.140625" style="96"/>
+    <col min="102" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" s="27" customFormat="1">
+    <row r="1" spans="1:101" s="27" customFormat="1" ht="30">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -54406,19 +54404,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B5:U75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:21" s="26" customFormat="1" ht="15" thickBot="1">
+    <row r="5" spans="2:21" s="26" customFormat="1" ht="15.75" thickBot="1">
       <c r="B5" s="26" t="s">
         <v>319</v>
       </c>
@@ -54516,7 +54514,7 @@
       <c r="T12" s="31"/>
       <c r="U12" s="37"/>
     </row>
-    <row r="13" spans="2:21" ht="15" thickBot="1">
+    <row r="13" spans="2:21" ht="15.75" thickBot="1">
       <c r="B13" s="20" t="s">
         <v>291</v>
       </c>
@@ -54550,7 +54548,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="19" spans="2:19" ht="15.5">
+    <row r="19" spans="2:19" ht="15.75">
       <c r="B19" s="21" t="s">
         <v>295</v>
       </c>
@@ -54568,7 +54566,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="22" spans="2:19" ht="15" thickBot="1">
+    <row r="22" spans="2:19" ht="15.75" thickBot="1">
       <c r="B22" s="18"/>
       <c r="N22" s="19" t="s">
         <v>392</v>
@@ -54633,7 +54631,7 @@
       <c r="R27" s="31"/>
       <c r="S27" s="37"/>
     </row>
-    <row r="28" spans="2:19" ht="15" thickBot="1">
+    <row r="28" spans="2:19" ht="15.75" thickBot="1">
       <c r="B28" s="20" t="s">
         <v>300</v>
       </c>
@@ -54786,12 +54784,12 @@
         <v>515</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="188.5">
+    <row r="67" spans="2:2" ht="195">
       <c r="B67" s="90" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="68" spans="2:2" ht="29">
+    <row r="68" spans="2:2" ht="30">
       <c r="B68" s="89" t="s">
         <v>517</v>
       </c>
@@ -54811,7 +54809,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="145">
+    <row r="72" spans="2:2" ht="150">
       <c r="B72" s="88" t="s">
         <v>519</v>
       </c>
@@ -54833,10 +54831,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B27" r:id="rId1" display="mailto:Jaimie.Potts@environment.nsw.gov.au"/>
-    <hyperlink ref="B29" r:id="rId2" display="mailto:Merran.Griffith@sydneywater.com.au"/>
-    <hyperlink ref="B38" r:id="rId3" display="mailto:Merran.Griffith@sydneywater.com.au"/>
-    <hyperlink ref="B40" r:id="rId4" display="mailto:Jaimie.Potts@environment.nsw.gov.au"/>
+    <hyperlink ref="B27" r:id="rId1" display="mailto:Jaimie.Potts@environment.nsw.gov.au" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B29" r:id="rId2" display="mailto:Merran.Griffith@sydneywater.com.au" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B38" r:id="rId3" display="mailto:Merran.Griffith@sydneywater.com.au" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B40" r:id="rId4" display="mailto:Jaimie.Potts@environment.nsw.gov.au" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -54844,14 +54842,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="Y50" sqref="Y50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>